<commit_message>
Update Scoring Metrics and Implement QC Functionality
This major update introduces the use of a reference retention time and CCS list, which may be used for simple quality control of internal standards (or other spiked standards). The scoring metrics for database matches are now more comprehensive and display cosine similarity, mass error, retention time error, and CCS error. This update also displays relevant information for each potential match (i.e., retention time and CCS) for accessibility.
</commit_message>
<xml_diff>
--- a/imms/expysomics/target_list_template.xlsx
+++ b/imms/expysomics/target_list_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/ryan97_uw_edu/Documents/QAC Metabolism/Manuscript Materials/RO1 Fecal Analysis/2023_07_27_RO1_pooled_feces/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/ryan97_uw_edu/Documents/Desktop/QAC Database Code/xulab_software/imms/expysomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{EA97EF42-8E36-4C04-957E-B60E08CC91EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5A0E741-38AA-2943-BAC9-B1DD270AB36A}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{EA97EF42-8E36-4C04-957E-B60E08CC91EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C66BEC2-CC40-432E-A4B2-D756E3B02B1C}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="2200" windowWidth="19320" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="1710" windowWidth="19440" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,24 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="13">
-  <si>
-    <t>file_name</t>
-  </si>
-  <si>
-    <t>mz</t>
-  </si>
-  <si>
-    <t>sample_type</t>
-  </si>
-  <si>
-    <t>ccs_calibrant</t>
-  </si>
-  <si>
-    <t>gradient</t>
-  </si>
-  <si>
-    <t>column_type</t>
-  </si>
   <si>
     <t>control</t>
   </si>
@@ -64,6 +46,24 @@
   </si>
   <si>
     <t>2023_07_27_004.raw</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Target m/z</t>
+  </si>
+  <si>
+    <t>Sample Type</t>
+  </si>
+  <si>
+    <t>CCS Calibrant</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>Column Type</t>
   </si>
 </sst>
 </file>
@@ -392,1121 +392,1121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>170.1909</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>172.20650000000001</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>186.1858</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>188.20140000000001</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>198.22219999999999</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>200.23779999999999</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>204.19630000000001</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>214.21709999999999</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
         <v>216.23269999999999</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
         <v>228.26910000000001</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
         <v>230.21199999999999</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1">
         <v>232.2276</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1">
         <v>242.2484</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>244.26400000000001</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
         <v>246.2217</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1">
         <v>248.2373</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1">
         <v>256.30040000000002</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
         <v>258.24329999999998</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1">
         <v>260.25889999999998</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1">
         <v>262.21660000000003</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1">
         <v>264.23219999999998</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1">
         <v>270.27969999999999</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1">
         <v>272.2953</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B25" s="1">
         <v>278.2115</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B26" s="1">
         <v>280.22710000000001</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1">
         <v>286.27460000000002</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1">
         <v>288.29020000000003</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1">
         <v>170.1909</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1">
         <v>172.20650000000001</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1">
         <v>186.1858</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1">
         <v>188.20140000000001</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1">
         <v>198.22219999999999</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1">
         <v>200.23779999999999</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1">
         <v>204.19630000000001</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B36" s="1">
         <v>214.21709999999999</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1">
         <v>216.23269999999999</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B38" s="1">
         <v>228.26910000000001</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1">
         <v>230.21199999999999</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1">
         <v>232.2276</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1">
         <v>242.2484</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1">
         <v>244.26400000000001</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1">
         <v>246.2217</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1">
         <v>248.2373</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B45" s="1">
         <v>256.30040000000002</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1">
         <v>258.24329999999998</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1">
         <v>260.25889999999998</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B48" s="1">
         <v>262.21660000000003</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1">
         <v>264.23219999999998</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1">
         <v>270.27969999999999</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1">
         <v>272.2953</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1">
         <v>278.2115</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B53" s="1">
         <v>280.22710000000001</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B54" s="1">
         <v>286.27460000000002</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1">
         <v>288.29020000000003</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1514,7 +1514,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1522,7 +1522,7 @@
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1530,7 +1530,7 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1538,7 +1538,7 @@
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1546,7 +1546,7 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1554,7 +1554,7 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1562,7 +1562,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1570,7 +1570,7 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1578,7 +1578,7 @@
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1586,7 +1586,7 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1594,7 +1594,7 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1602,7 +1602,7 @@
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1610,7 +1610,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1618,7 +1618,7 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1626,7 +1626,7 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1634,7 +1634,7 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1642,7 +1642,7 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1650,7 +1650,7 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1658,7 +1658,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1666,7 +1666,7 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1674,7 +1674,7 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1682,7 +1682,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1690,7 +1690,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1698,7 +1698,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1706,7 +1706,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1714,7 +1714,7 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1722,7 +1722,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1730,7 +1730,7 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1738,7 +1738,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1746,7 +1746,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1754,7 +1754,7 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1762,7 +1762,7 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1770,7 +1770,7 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1778,7 +1778,7 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1786,7 +1786,7 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1794,7 +1794,7 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1802,7 +1802,7 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1810,7 +1810,7 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1818,7 +1818,7 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1826,7 +1826,7 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1834,7 +1834,7 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1842,7 +1842,7 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1850,7 +1850,7 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1858,7 +1858,7 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1866,7 +1866,7 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1874,7 +1874,7 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1882,7 +1882,7 @@
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1890,7 +1890,7 @@
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1898,7 +1898,7 @@
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1906,7 +1906,7 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1914,7 +1914,7 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1922,7 +1922,7 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1930,7 +1930,7 @@
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1938,7 +1938,7 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1946,7 +1946,7 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1954,7 +1954,7 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1962,7 +1962,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -1970,7 +1970,7 @@
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -1978,7 +1978,7 @@
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1986,7 +1986,7 @@
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -1994,7 +1994,7 @@
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2002,7 +2002,7 @@
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2010,7 +2010,7 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2018,7 +2018,7 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2026,7 +2026,7 @@
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2034,7 +2034,7 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2042,7 +2042,7 @@
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2050,7 +2050,7 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2058,7 +2058,7 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2066,7 +2066,7 @@
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2074,7 +2074,7 @@
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2082,7 +2082,7 @@
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2090,7 +2090,7 @@
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2098,7 +2098,7 @@
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2106,7 +2106,7 @@
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2114,7 +2114,7 @@
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2122,7 +2122,7 @@
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2130,7 +2130,7 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2138,7 +2138,7 @@
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2146,7 +2146,7 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2154,7 +2154,7 @@
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2162,7 +2162,7 @@
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2170,7 +2170,7 @@
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2178,7 +2178,7 @@
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2186,7 +2186,7 @@
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2194,7 +2194,7 @@
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -2202,7 +2202,7 @@
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -2210,7 +2210,7 @@
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -2218,7 +2218,7 @@
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -2226,7 +2226,7 @@
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -2234,7 +2234,7 @@
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -2242,7 +2242,7 @@
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2250,7 +2250,7 @@
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2258,7 +2258,7 @@
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2266,7 +2266,7 @@
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2274,7 +2274,7 @@
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2282,7 +2282,7 @@
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2290,7 +2290,7 @@
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2298,7 +2298,7 @@
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2306,7 +2306,7 @@
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2314,7 +2314,7 @@
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2322,7 +2322,7 @@
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2330,7 +2330,7 @@
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2338,7 +2338,7 @@
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2346,7 +2346,7 @@
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2354,7 +2354,7 @@
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2362,7 +2362,7 @@
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>

</xml_diff>